<commit_message>
Test failed screenshot added
Change-Id: I424f7d583f73f42f23e7d5e3729790c0feff26a4
Signed-off-by: IrappaH <irappahukkeri@gmail.com>
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5377B83B-33F7-49E8-AF19-1915350AE2EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EB61BBA0-749E-4E10-BCD7-706EEBB77FB4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -107,10 +108,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,12 +397,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -418,7 +423,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -434,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB2EC91-78A9-4C92-A788-8695057AA27D}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,4 +502,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C1FD22-644E-4B3C-8F82-566A64C42B71}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Microsoft drivers Modified interface constants values Modified pom class
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EB61BBA0-749E-4E10-BCD7-706EEBB77FB4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D1A265E2-DCEA-473B-8F30-98C4A389D622}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added multiple user for login page
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D1A265E2-DCEA-473B-8F30-98C4A389D622}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{38E06D90-44D0-46F9-A4F7-F8A57ABB964B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>User name</t>
   </si>
@@ -36,22 +36,22 @@
     <t>uswm</t>
   </si>
   <si>
+    <t>uswm1</t>
+  </si>
+  <si>
+    <t>wer</t>
+  </si>
+  <si>
+    <t>Invalid User Name/Password !</t>
+  </si>
+  <si>
+    <t>Please enter password!</t>
+  </si>
+  <si>
+    <t>Please enter user name!</t>
+  </si>
+  <si>
     <t>WaterConsumption | Liter</t>
-  </si>
-  <si>
-    <t>uswm1</t>
-  </si>
-  <si>
-    <t>wer</t>
-  </si>
-  <si>
-    <t>Invalid User Name/Password !</t>
-  </si>
-  <si>
-    <t>Please enter password!</t>
-  </si>
-  <si>
-    <t>Please enter user name!</t>
   </si>
 </sst>
 </file>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,62 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -463,39 +518,39 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J5" s="1">
         <v>16</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>